<commit_message>
update member pay fee
</commit_message>
<xml_diff>
--- a/Vinasa/Content/Files/MauDongPhi.xlsx
+++ b/Vinasa/Content/Files/MauDongPhi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HK3_NH21-22\SEP\fixcode\Vinasa\Vinasa\Content\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HK3_NH21-22\SEP\Vinasa\Vinasa\Content\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92874B75-CBCE-4CEE-B9FE-F638BAADC790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D5DED3-7CBE-4433-B78B-C5EBF2BF4AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{E7D69EFB-3D21-42E6-B5B6-1781657AD360}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">Mã số thuế </t>
   </si>
@@ -64,13 +64,19 @@
   <si>
     <t>Ngày gửi phiếu thu
 (Theo định dạng mm/dd/yyyy)</t>
+  </si>
+  <si>
+    <t>Địa chỉ ghi trên Phiếu thu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Địa chỉ gửi phiếu thu </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +105,13 @@
       <family val="1"/>
       <charset val="163"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -126,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -138,6 +151,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -454,25 +470,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F675F848-DDA6-41ED-85E1-4B4A0DEA1D6C}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
@@ -482,32 +500,40 @@
       <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>